<commit_message>
Updated Google Drive data 2020-10-22
</commit_message>
<xml_diff>
--- a/Google Drive Mirror/RCOS Resources/Status Updates.xlsx
+++ b/Google Drive Mirror/RCOS Resources/Status Updates.xlsx
@@ -78,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -88,9 +88,10 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -122,12 +123,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -394,7 +389,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3"/>
@@ -556,7 +551,7 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3"/>
@@ -588,7 +583,7 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3"/>
@@ -620,7 +615,7 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3"/>
@@ -677,7 +672,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -705,7 +700,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -733,7 +728,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>

</xml_diff>

<commit_message>
Updated Google Drive data 2021-01-27
</commit_message>
<xml_diff>
--- a/Google Drive Mirror/RCOS Resources/Status Updates.xlsx
+++ b/Google Drive Mirror/RCOS Resources/Status Updates.xlsx
@@ -78,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -88,10 +88,9 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -123,6 +122,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -389,7 +394,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3"/>
@@ -551,7 +556,7 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3"/>
@@ -583,7 +588,7 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3"/>
@@ -615,7 +620,7 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3"/>
@@ -672,7 +677,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -700,7 +705,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -728,7 +733,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>

</xml_diff>